<commit_message>
Fix: Formulas corregidas al 100%
</commit_message>
<xml_diff>
--- a/storage/app/plantilla/Formulas.xlsx
+++ b/storage/app/plantilla/Formulas.xlsx
@@ -2761,21 +2761,21 @@
       <c r="G14" s="66" t="n"/>
       <c r="H14" s="5" t="n"/>
       <c r="I14" s="68">
-        <f>IFERROR(MIN(H14/G14, 1), 0)</f>
+        <f>IFERROR(MIN(H14/G14, 1), "0%")</f>
         <v/>
       </c>
       <c r="J14" s="131" t="n"/>
       <c r="K14" s="69" t="n"/>
       <c r="L14" s="6" t="n"/>
       <c r="M14" s="68">
-        <f>IFERROR(MIN(L14/K14, 1), 0)</f>
+        <f>IFERROR(MIN(L14/K14, 1), "0%")</f>
         <v/>
       </c>
       <c r="N14" s="7" t="n"/>
       <c r="O14" s="67" t="n"/>
       <c r="P14" s="6" t="n"/>
       <c r="Q14" s="68">
-        <f>IFERROR(MIN(P14/O14, 1), 0)</f>
+        <f>IFERROR(MIN(P14/O14, 1), "0%")</f>
         <v/>
       </c>
       <c r="R14" s="7" t="n"/>
@@ -2786,21 +2786,21 @@
       <c r="T14" s="69" t="n"/>
       <c r="U14" s="11" t="n"/>
       <c r="V14" s="68">
-        <f>IFERROR(MIN(U14/T14, 1), 0)</f>
+        <f>IFERROR(MIN(U14/T14, 1), "0%")</f>
         <v/>
       </c>
       <c r="W14" s="131" t="n"/>
       <c r="X14" s="69" t="n"/>
       <c r="Y14" s="11" t="n"/>
       <c r="Z14" s="68">
-        <f>IFERROR(MIN(Y14/X14, 1), 0)</f>
+        <f>IFERROR(MIN(Y14/X14, 1), "0%")</f>
         <v/>
       </c>
       <c r="AA14" s="131" t="n"/>
       <c r="AB14" s="69" t="n"/>
       <c r="AC14" s="11" t="n"/>
       <c r="AD14" s="68">
-        <f>IFERROR(MIN(AC14/AB14, 1), 0)</f>
+        <f>IFERROR(MIN(AC14/AB14, 1), "0%")</f>
         <v/>
       </c>
       <c r="AE14" s="133" t="n"/>
@@ -2815,21 +2815,21 @@
       <c r="AH14" s="73" t="n"/>
       <c r="AI14" s="134" t="n"/>
       <c r="AJ14" s="75">
-        <f>IFERROR(MIN(AI14/AH14, 1), 0)</f>
+        <f>IFERROR(MIN(AI14/AH14, 1), "0%")</f>
         <v/>
       </c>
       <c r="AK14" s="133" t="n"/>
       <c r="AL14" s="74" t="n"/>
       <c r="AM14" s="134" t="n"/>
       <c r="AN14" s="75">
-        <f>IFERROR(MIN(AM14/AL14, 1), 0)</f>
+        <f>IFERROR(MIN(AM14/AL14, 1), "0%")</f>
         <v/>
       </c>
       <c r="AO14" s="133" t="n"/>
       <c r="AP14" s="74" t="n"/>
       <c r="AQ14" s="134" t="n"/>
       <c r="AR14" s="75">
-        <f>IFERROR(MIN(AQ14/AP14, 1), 0)</f>
+        <f>IFERROR(MIN(AQ14/AP14, 1), "0%")</f>
         <v/>
       </c>
       <c r="AS14" s="133" t="n"/>
@@ -2840,21 +2840,21 @@
       <c r="AU14" s="74" t="n"/>
       <c r="AV14" s="134" t="n"/>
       <c r="AW14" s="75">
-        <f>IFERROR(MIN(AV14/AU14, 1), 0)</f>
+        <f>IFERROR(MIN(AV14/AU14, 1), "0%")</f>
         <v/>
       </c>
       <c r="AX14" s="133" t="n"/>
       <c r="AY14" s="74" t="n"/>
       <c r="AZ14" s="134" t="n"/>
       <c r="BA14" s="75">
-        <f>IFERROR(MIN(AZ14/AY14, 1), 0)</f>
+        <f>IFERROR(MIN(AZ14/AY14, 1), "0%")</f>
         <v/>
       </c>
       <c r="BB14" s="133" t="n"/>
       <c r="BC14" s="74" t="n"/>
       <c r="BD14" s="134" t="n"/>
       <c r="BE14" s="75">
-        <f>IFERROR(MIN(BD14/BC14, 1), 0)</f>
+        <f>IFERROR(MIN(BD14/BC14, 1), "0%")</f>
         <v/>
       </c>
       <c r="BF14" s="135" t="n"/>
@@ -4799,7 +4799,6 @@
   </sheetData>
   <mergeCells count="18">
     <mergeCell ref="D10:D13"/>
-    <mergeCell ref="G10:BI10"/>
     <mergeCell ref="O12:R12"/>
     <mergeCell ref="E10:E13"/>
     <mergeCell ref="T12:W12"/>
@@ -4813,9 +4812,10 @@
     <mergeCell ref="AH12:AK12"/>
     <mergeCell ref="K12:N12"/>
     <mergeCell ref="AU12:AX12"/>
+    <mergeCell ref="F10:F13"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="B10:B13"/>
-    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="G10:BI10"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.1968503937007874" right="0.1968503937007874" top="0.1968503937007874" bottom="0.1968503937007874" header="0.3149606299212598" footer="0.3149606299212598"/>

</xml_diff>